<commit_message>
added normalization to series files
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\MEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Documents\git\MEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E60980C-2247-4102-9B2B-6800219D8D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389F368-A02B-4029-9579-9A43DAD45E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="84">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>node1_wind</t>
+  </si>
+  <si>
+    <t>normalization</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -375,6 +378,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3758,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735D713C-0288-4607-850D-121F4BB78710}">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3871,7 +3877,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -3883,7 +3889,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -3895,7 +3901,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3907,7 +3913,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -3919,7 +3925,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -3931,7 +3937,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
@@ -3943,10 +3949,10 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
@@ -3960,8 +3966,9 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="10"/>
       <c r="C25" s="7"/>
@@ -3973,8 +3980,9 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -3990,8 +3998,9 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>46</v>
       </c>
@@ -4007,8 +4016,9 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>47</v>
       </c>
@@ -4024,8 +4034,9 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>48</v>
       </c>
@@ -4039,8 +4050,9 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>50</v>
       </c>
@@ -4056,8 +4068,9 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>51</v>
       </c>
@@ -4073,8 +4086,9 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>52</v>
       </c>
@@ -4090,8 +4104,9 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="7"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>53</v>
       </c>
@@ -4107,8 +4122,9 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="7"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>54</v>
       </c>
@@ -4124,8 +4140,9 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="7"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>55</v>
       </c>
@@ -4141,8 +4158,9 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="7"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>56</v>
       </c>
@@ -4158,8 +4176,9 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="7"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>57</v>
       </c>
@@ -4175,8 +4194,9 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>49</v>
       </c>
@@ -4192,8 +4212,9 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="7"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -4205,8 +4226,9 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="7"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>44</v>
       </c>
@@ -4220,8 +4242,9 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -4233,8 +4256,9 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-    </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L41" s="7"/>
+    </row>
+    <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>1</v>
       </c>
@@ -4251,25 +4275,28 @@
         <v>5</v>
       </c>
       <c r="F42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="K42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="L42" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -4284,14 +4311,17 @@
         <v>58</v>
       </c>
       <c r="F43" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G43" s="2">
         <v>0.03</v>
       </c>
-      <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
@@ -4307,8 +4337,9 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -4321,13 +4352,16 @@
       <c r="E45" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="15">
+        <v>1</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -4340,14 +4374,15 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2">
         <v>10</v>
       </c>
-      <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -4359,17 +4394,18 @@
         <v>26</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="2">
-        <v>0.02</v>
-      </c>
+      <c r="F47" s="2"/>
       <c r="G47" s="2">
         <v>0.02</v>
       </c>
-      <c r="H47" s="2"/>
+      <c r="H47" s="2">
+        <v>0.02</v>
+      </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -4383,19 +4419,20 @@
         <v>26</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="2">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2">
         <v>0.01</v>
       </c>
-      <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="I48" s="2">
+      <c r="I48" s="2"/>
+      <c r="J48" s="2">
         <v>0.9</v>
       </c>
-      <c r="J48" s="2">
+      <c r="K48" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -4409,22 +4446,23 @@
         <v>19</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="2">
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
         <v>0.02</v>
       </c>
-      <c r="G49" s="2">
+      <c r="H49" s="2">
         <v>0.01</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2">
+      <c r="I49" s="2"/>
+      <c r="J49" s="2">
         <v>0.9</v>
       </c>
-      <c r="J49" s="2"/>
-      <c r="K49" t="s">
+      <c r="K49" s="2"/>
+      <c r="L49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -4437,13 +4475,16 @@
       <c r="E50" t="s">
         <v>61</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -4456,14 +4497,15 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2">
+      <c r="G51" s="2"/>
+      <c r="H51" s="2">
         <v>10</v>
       </c>
-      <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>40</v>
       </c>
@@ -4476,13 +4518,16 @@
       <c r="E52" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -4497,14 +4542,17 @@
         <v>60</v>
       </c>
       <c r="F53" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G53" s="2">
         <v>0.03</v>
       </c>
-      <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
@@ -4520,8 +4568,9 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -4535,22 +4584,23 @@
         <v>41</v>
       </c>
       <c r="E55" s="2"/>
-      <c r="F55" s="2">
-        <v>0.01</v>
-      </c>
+      <c r="F55" s="2"/>
       <c r="G55" s="2">
         <v>0.01</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2">
+      <c r="H55" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2">
         <v>0.9</v>
       </c>
-      <c r="J55" s="2"/>
-      <c r="K55" t="s">
+      <c r="K55" s="2"/>
+      <c r="L55" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4563,14 +4613,15 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2">
+      <c r="G56" s="2"/>
+      <c r="H56" s="2">
         <v>10</v>
       </c>
-      <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -4579,8 +4630,9 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>45</v>
       </c>
@@ -4594,10 +4646,11 @@
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="9"/>
       <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -4610,7 +4663,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4623,7 +4676,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4636,7 +4689,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4649,7 +4702,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4662,7 +4715,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>

</xml_diff>

<commit_message>
Update demand and wind and solar files used in example script
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfarnham/Google Drive/MEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/MEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0B1260-63C7-D244-84D0-465CE967862E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104779CC-5B1E-4640-A1AA-8B63C041E26D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="24880" windowHeight="17540" activeTab="4" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
+    <workbookView xWindow="-3820" yWindow="-25380" windowWidth="38020" windowHeight="24600" activeTab="5" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
   <sheets>
     <sheet name="simplest_example" sheetId="3" r:id="rId1"/>
@@ -202,21 +202,9 @@
     <t>hour_end</t>
   </si>
   <si>
-    <t>solar_series_Shaner_normalized_to_0.2_mean.csv</t>
-  </si>
-  <si>
     <t>node_3_wind</t>
   </si>
   <si>
-    <t>wind_series_Shaner_normalized_to_0.38_mean.csv</t>
-  </si>
-  <si>
-    <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
-  </si>
-  <si>
-    <t>Input_Data/Shaner-et-al_E&amp;ES2018</t>
-  </si>
-  <si>
     <t>test_case</t>
   </si>
   <si>
@@ -290,6 +278,18 @@
   </si>
   <si>
     <t>Option to specify the capacity of a technology. If this number is supplied, then the technology capacity is fixed and is not included as a decision variable in the optimization</t>
+  </si>
+  <si>
+    <t>Input_Data/Lei_Solar_Wind</t>
+  </si>
+  <si>
+    <t>US_demand_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_solar_threshold26_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_wind_threshold26_unnormalized.csv</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -769,7 +769,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -793,7 +793,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -832,10 +832,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -845,10 +845,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -900,7 +900,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -957,7 +957,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -974,7 +974,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -991,7 +991,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -1023,7 +1023,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1091,7 +1091,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1220,10 +1220,10 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -1244,12 +1244,12 @@
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
         <v>29</v>
@@ -1271,10 +1271,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -1299,7 +1299,7 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1489,7 +1489,7 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD24"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1557,7 +1557,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1633,10 +1633,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1688,7 +1688,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1745,7 +1745,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1762,7 +1762,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1779,7 +1779,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -1811,7 +1811,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1879,7 +1879,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -2008,10 +2008,10 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -2032,22 +2032,22 @@
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F45" s="2">
         <v>0.04</v>
@@ -2076,10 +2076,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>24</v>
@@ -2104,7 +2104,7 @@
         <v>24</v>
       </c>
       <c r="E48" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>17</v>
@@ -2309,7 +2309,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD24"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2377,7 +2377,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2401,7 +2401,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -2440,10 +2440,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2453,10 +2453,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2508,7 +2508,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2565,7 +2565,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2582,7 +2582,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2599,7 +2599,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -2631,7 +2631,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -2699,7 +2699,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -2828,10 +2828,10 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -2852,22 +2852,22 @@
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F45" s="2">
         <v>0.04</v>
@@ -2888,7 +2888,7 @@
         <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2898,10 +2898,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
@@ -3119,7 +3119,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD24"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3187,7 +3187,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -3224,7 +3224,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -3250,10 +3250,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3263,10 +3263,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3318,7 +3318,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3375,7 +3375,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -3392,7 +3392,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -3409,7 +3409,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -3441,7 +3441,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -3509,7 +3509,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -3638,10 +3638,10 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -3662,12 +3662,12 @@
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
         <v>29</v>
@@ -3689,10 +3689,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -3717,7 +3717,7 @@
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3921,8 +3921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735D713C-0288-4607-850D-121F4BB78710}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3991,7 +3991,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -4054,10 +4054,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4067,10 +4067,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4122,7 +4122,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4183,7 +4183,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -4202,7 +4202,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -4221,7 +4221,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -4257,7 +4257,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -4333,7 +4333,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -4478,19 +4478,19 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>9</v>
@@ -4508,7 +4508,7 @@
         <v>13</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -4516,14 +4516,14 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F45" s="2">
         <v>0.2</v>
@@ -4567,7 +4567,7 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F47" s="15">
         <v>1</v>
@@ -4581,10 +4581,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
@@ -4655,7 +4655,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>31</v>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="L51" s="2"/>
       <c r="M51" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
         <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -4709,10 +4709,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
@@ -4740,7 +4740,7 @@
         <v>37</v>
       </c>
       <c r="E54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -4754,17 +4754,17 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F55" s="2">
         <v>0.38</v>
@@ -4780,7 +4780,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>27</v>
@@ -4799,10 +4799,10 @@
     </row>
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>17</v>
@@ -4825,15 +4825,15 @@
       </c>
       <c r="L57" s="2"/>
       <c r="M57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
@@ -5032,8 +5032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA16AE9-162C-4BF3-B3D7-7E425583483C}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44:G58"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5101,7 +5101,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>33</v>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
@@ -5164,10 +5164,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -5177,10 +5177,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -5232,7 +5232,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -5293,7 +5293,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -5312,7 +5312,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -5331,7 +5331,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -5367,7 +5367,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -5443,7 +5443,7 @@
         <v>50</v>
       </c>
       <c r="B36" s="12">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -5588,19 +5588,19 @@
         <v>26</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>9</v>
@@ -5618,7 +5618,7 @@
         <v>13</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -5626,14 +5626,14 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F45" s="2">
         <v>0.2</v>
@@ -5677,7 +5677,7 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F47" s="15">
         <v>1</v>
@@ -5691,10 +5691,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
@@ -5767,7 +5767,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>31</v>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="L51" s="2"/>
       <c r="M51" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -5807,7 +5807,7 @@
         <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -5821,10 +5821,10 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
@@ -5852,7 +5852,7 @@
         <v>37</v>
       </c>
       <c r="E54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -5866,17 +5866,17 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F55" s="2">
         <v>0.38</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>27</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>17</v>
@@ -5937,15 +5937,15 @@
       </c>
       <c r="L57" s="2"/>
       <c r="M57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">

</xml_diff>

<commit_message>
add fixed and var prices for CO2 emissions
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/MEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfarnham/Google Drive/MEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104779CC-5B1E-4640-A1AA-8B63C041E26D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C82F1-F340-9949-8904-DA91C54FAD04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3820" yWindow="-25380" windowWidth="38020" windowHeight="24600" activeTab="5" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="33120" windowHeight="20540" activeTab="6" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
   <sheets>
     <sheet name="simplest_example" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="simplest_example2" sheetId="4" r:id="rId4"/>
     <sheet name="case_input_example" sheetId="1" r:id="rId5"/>
     <sheet name="case_input_capacity" sheetId="7" r:id="rId6"/>
+    <sheet name="case_input_co2_price" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="89">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -106,9 +107,6 @@
     <t>node_2_natgas</t>
   </si>
   <si>
-    <t>node1_solar</t>
-  </si>
-  <si>
     <t>Note that demand has no decisions.</t>
   </si>
   <si>
@@ -256,12 +254,6 @@
     <t>node_to</t>
   </si>
   <si>
-    <t>node1_natgas</t>
-  </si>
-  <si>
-    <t>node1_wind</t>
-  </si>
-  <si>
     <t>normalization</t>
   </si>
   <si>
@@ -290,6 +282,30 @@
   </si>
   <si>
     <t>US_capacity_wind_threshold26_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>node_1_natgas</t>
+  </si>
+  <si>
+    <t>node_1_wind</t>
+  </si>
+  <si>
+    <t>node_1_solar</t>
+  </si>
+  <si>
+    <t>co2_price</t>
+  </si>
+  <si>
+    <t>var_co2</t>
+  </si>
+  <si>
+    <t>fixed_co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate of CO_2 emissions when consuming fuel (kg CO_2/kWh) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate of CO_2 emissions when buidling capacity of a generator (kg CO_2/kW) </t>
   </si>
 </sst>
 </file>
@@ -700,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1CB86B-8C48-416D-A7E1-B75D92C9D066}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -732,7 +748,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -766,10 +782,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -793,10 +809,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -806,10 +822,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -832,10 +848,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -845,10 +861,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -897,10 +913,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -926,7 +942,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -954,10 +970,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -971,10 +987,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -988,10 +1004,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -1005,7 +1021,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -1020,7 +1036,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -1037,7 +1053,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -1054,7 +1070,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -1071,7 +1087,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -1088,7 +1104,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -1105,7 +1121,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -1122,7 +1138,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -1139,7 +1155,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -1156,7 +1172,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -1186,7 +1202,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -1217,13 +1233,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -1238,21 +1254,21 @@
         <v>11</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
@@ -1271,10 +1287,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -1293,13 +1309,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1320,7 +1336,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="9"/>
@@ -1489,7 +1505,7 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1520,7 +1536,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1554,10 +1570,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1581,10 +1597,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1594,10 +1610,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1620,10 +1636,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1633,10 +1649,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1685,10 +1701,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1714,7 +1730,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -1742,10 +1758,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1759,10 +1775,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1776,10 +1792,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -1793,7 +1809,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -1808,7 +1824,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -1825,7 +1841,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -1842,7 +1858,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -1859,7 +1875,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -1876,7 +1892,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -1893,7 +1909,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -1910,7 +1926,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -1927,7 +1943,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -1944,7 +1960,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -1974,7 +1990,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -2005,13 +2021,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -2026,28 +2042,28 @@
         <v>11</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F45" s="2">
         <v>0.04</v>
@@ -2062,7 +2078,7 @@
         <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>17</v>
@@ -2076,13 +2092,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -2095,16 +2111,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -2114,16 +2130,16 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
@@ -2140,7 +2156,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="9"/>
@@ -2309,7 +2325,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2340,7 +2356,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2374,10 +2390,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2401,10 +2417,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2414,10 +2430,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2440,10 +2456,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2453,10 +2469,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2505,10 +2521,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2534,7 +2550,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -2562,10 +2578,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2579,10 +2595,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2596,10 +2612,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -2613,7 +2629,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -2628,7 +2644,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -2645,7 +2661,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -2662,7 +2678,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -2679,7 +2695,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -2696,7 +2712,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -2713,7 +2729,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -2730,7 +2746,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -2747,7 +2763,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -2764,7 +2780,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -2794,7 +2810,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -2825,13 +2841,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -2846,28 +2862,28 @@
         <v>11</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F45" s="2">
         <v>0.04</v>
@@ -2879,16 +2895,16 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2898,16 +2914,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2">
@@ -2924,16 +2940,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2">
@@ -2950,7 +2966,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="9"/>
@@ -3119,7 +3135,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3150,7 +3166,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3184,10 +3200,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -3211,10 +3227,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3224,10 +3240,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3250,10 +3266,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3263,10 +3279,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3315,10 +3331,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3344,7 +3360,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -3372,10 +3388,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -3389,10 +3405,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -3406,10 +3422,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -3423,7 +3439,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -3438,7 +3454,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -3455,7 +3471,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -3472,7 +3488,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -3489,7 +3505,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -3506,7 +3522,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -3523,7 +3539,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -3540,7 +3556,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -3557,7 +3573,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -3574,7 +3590,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -3604,7 +3620,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -3635,13 +3651,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
@@ -3656,21 +3672,21 @@
         <v>11</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
@@ -3689,10 +3705,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -3708,16 +3724,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -3727,16 +3743,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2">
@@ -3753,7 +3769,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="9"/>
@@ -3921,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735D713C-0288-4607-850D-121F4BB78710}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3954,7 +3970,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3988,10 +4004,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4015,10 +4031,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -4028,10 +4044,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -4054,10 +4070,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4067,10 +4083,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4119,10 +4135,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4148,7 +4164,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -4180,10 +4196,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -4199,10 +4215,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -4218,10 +4234,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -4237,7 +4253,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -4254,7 +4270,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -4273,7 +4289,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -4292,7 +4308,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -4311,7 +4327,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -4330,7 +4346,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -4349,7 +4365,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -4368,7 +4384,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>2</v>
@@ -4387,7 +4403,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -4406,7 +4422,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -4440,7 +4456,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -4475,22 +4491,22 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>9</v>
@@ -4502,28 +4518,28 @@
         <v>11</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F45" s="2">
         <v>0.2</v>
@@ -4542,7 +4558,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>17</v>
@@ -4561,13 +4577,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F47" s="15">
         <v>1</v>
@@ -4581,10 +4597,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
@@ -4606,11 +4622,11 @@
         <v>21</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -4627,16 +4643,16 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -4655,13 +4671,13 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>17</v>
@@ -4681,21 +4697,21 @@
       </c>
       <c r="L51" s="2"/>
       <c r="M51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -4709,14 +4725,14 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -4731,16 +4747,16 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -4754,17 +4770,17 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F55" s="2">
         <v>0.38</v>
@@ -4780,13 +4796,13 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -4799,16 +4815,16 @@
     </row>
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -4825,19 +4841,19 @@
       </c>
       <c r="L57" s="2"/>
       <c r="M57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -4863,7 +4879,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="9"/>
@@ -5032,8 +5048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA16AE9-162C-4BF3-B3D7-7E425583483C}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5064,7 +5080,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5098,10 +5114,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -5125,10 +5141,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -5138,10 +5154,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5164,10 +5180,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -5177,10 +5193,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -5229,10 +5245,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -5258,7 +5274,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
@@ -5290,10 +5306,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -5309,10 +5325,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -5328,10 +5344,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
@@ -5347,7 +5363,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="7"/>
@@ -5364,7 +5380,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="12">
         <v>2017</v>
@@ -5383,7 +5399,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -5402,7 +5418,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="12">
         <v>1</v>
@@ -5421,7 +5437,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -5440,7 +5456,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="12">
         <v>2017</v>
@@ -5459,7 +5475,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -5478,7 +5494,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="12">
         <v>2</v>
@@ -5497,7 +5513,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="12">
         <v>24</v>
@@ -5516,7 +5532,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="13">
         <v>9.9999999999999998E+23</v>
@@ -5550,7 +5566,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -5585,22 +5601,22 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>9</v>
@@ -5612,28 +5628,28 @@
         <v>11</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F45" s="2">
         <v>0.2</v>
@@ -5652,7 +5668,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>17</v>
@@ -5671,13 +5687,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F47" s="15">
         <v>1</v>
@@ -5691,10 +5707,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
@@ -5716,11 +5732,11 @@
         <v>21</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -5739,16 +5755,16 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -5767,13 +5783,13 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>17</v>
@@ -5793,21 +5809,21 @@
       </c>
       <c r="L51" s="2"/>
       <c r="M51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -5821,14 +5837,14 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -5843,16 +5859,16 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -5866,17 +5882,17 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F55" s="2">
         <v>0.38</v>
@@ -5892,13 +5908,13 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -5911,16 +5927,16 @@
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -5937,19 +5953,19 @@
       </c>
       <c r="L57" s="2"/>
       <c r="M57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -5976,7 +5992,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="9"/>
@@ -6151,4 +6167,1220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428C295-1449-B942-94DE-B4DC493F45AE}">
+  <dimension ref="A1:O74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" customWidth="1"/>
+    <col min="6" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="12">
+        <v>2017</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="12">
+        <v>2017</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="12">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="12">
+        <v>24</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="13">
+        <v>9.9999999999999998E+23</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+    </row>
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="15">
+        <v>1</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2">
+        <v>10</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2">
+        <v>0.46100000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L53" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L54" s="2"/>
+      <c r="O54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2">
+        <v>10</v>
+      </c>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L60" s="2"/>
+      <c r="O60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2">
+        <v>10</v>
+      </c>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add fixed_co2 option for transfer, transmission, and storage
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfarnham/Google Drive/MEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C82F1-F340-9949-8904-DA91C54FAD04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD96AE1-8C89-4643-A53D-78EF85C9D276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="33120" windowHeight="20540" activeTab="6" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
@@ -305,7 +305,7 @@
     <t xml:space="preserve">Rate of CO_2 emissions when consuming fuel (kg CO_2/kWh) </t>
   </si>
   <si>
-    <t xml:space="preserve">Rate of CO_2 emissions when buidling capacity of a generator (kg CO_2/kW) </t>
+    <t xml:space="preserve">Rate of CO_2 emissions when buidling capacity (the units are kg CO_2/kW for generators, transfers, and transmission; the units are kg CO_2/kWh for storage) </t>
   </si>
 </sst>
 </file>
@@ -6173,7 +6173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428C295-1449-B942-94DE-B4DC493F45AE}">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add ability to specify a max installed capacity per tech
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfarnham/Google Drive/MEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/MEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD96AE1-8C89-4643-A53D-78EF85C9D276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3307D8A-2A6F-6943-92B1-6D77FB88995E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="33120" windowHeight="20540" activeTab="6" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
+    <workbookView xWindow="5140" yWindow="-23680" windowWidth="31760" windowHeight="21920" activeTab="7" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
   <sheets>
     <sheet name="simplest_example" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="case_input_example" sheetId="1" r:id="rId5"/>
     <sheet name="case_input_capacity" sheetId="7" r:id="rId6"/>
     <sheet name="case_input_co2_price" sheetId="9" r:id="rId7"/>
+    <sheet name="case_input_max_capacity" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="94">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -306,13 +307,28 @@
   </si>
   <si>
     <t xml:space="preserve">Rate of CO_2 emissions when buidling capacity (the units are kg CO_2/kW for generators, transfers, and transmission; the units are kg CO_2/kWh for storage) </t>
+  </si>
+  <si>
+    <t>max_capacity</t>
+  </si>
+  <si>
+    <t>node_1_solar1</t>
+  </si>
+  <si>
+    <t>node_1_solar2</t>
+  </si>
+  <si>
+    <t>node_1_wind1</t>
+  </si>
+  <si>
+    <t>node_1_wind2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +340,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,6 +421,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -717,7 +746,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="A45" sqref="A45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6173,8 +6202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428C295-1449-B942-94DE-B4DC493F45AE}">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="O18" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7383,4 +7412,1096 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3228D5-8C52-004C-AB7F-D57B454DC51F}">
+  <dimension ref="A1:P68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" customWidth="1"/>
+    <col min="6" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="12">
+        <v>2017</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="12">
+        <v>2017</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="12">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="12">
+        <v>24</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="13">
+        <v>9.9999999999999998E+23</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+    </row>
+    <row r="47" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="P47" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="17">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="O48">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="16">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="17">
+        <v>0.159</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="O50">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="17">
+        <v>0.159</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="H52" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="O52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="15">
+        <v>1</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2">
+        <v>10</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit on 26 June 2024.
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/MEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacquelinedowling/MEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3307D8A-2A6F-6943-92B1-6D77FB88995E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55161FA-7D18-B24D-9E42-9770954BE25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="-23680" windowWidth="31760" windowHeight="21920" activeTab="7" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="simplest_example" sheetId="3" r:id="rId1"/>
-    <sheet name="simple_example2" sheetId="5" r:id="rId2"/>
-    <sheet name="simple_example3" sheetId="6" r:id="rId3"/>
-    <sheet name="simplest_example2" sheetId="4" r:id="rId4"/>
-    <sheet name="case_input_example" sheetId="1" r:id="rId5"/>
-    <sheet name="case_input_capacity" sheetId="7" r:id="rId6"/>
-    <sheet name="case_input_co2_price" sheetId="9" r:id="rId7"/>
-    <sheet name="case_input_max_capacity" sheetId="10" r:id="rId8"/>
+    <sheet name="natgas_alone" sheetId="11" r:id="rId1"/>
+    <sheet name="simplest_example" sheetId="3" r:id="rId2"/>
+    <sheet name="simple_example2" sheetId="5" r:id="rId3"/>
+    <sheet name="simple_example3" sheetId="6" r:id="rId4"/>
+    <sheet name="simplest_example2" sheetId="4" r:id="rId5"/>
+    <sheet name="case_input_example" sheetId="1" r:id="rId6"/>
+    <sheet name="case_input_capacity" sheetId="7" r:id="rId7"/>
+    <sheet name="case_input_co2_price" sheetId="9" r:id="rId8"/>
+    <sheet name="case_input_max_capacity" sheetId="10" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="HOURS_PER_YEAR">natgas_alone!$B$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="94">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -390,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -429,6 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,11 +747,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1CB86B-8C48-416D-A7E1-B75D92C9D066}">
-  <dimension ref="A1:M60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8256C-66F1-2E46-B889-4870D3A8C883}">
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1067,6 +1072,779 @@
       <c r="A32" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="B32">
+        <v>2017</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36">
+        <v>2017</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38">
+        <v>31</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="18">
+        <v>9.9999999999999998E+23</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2">
+        <f>10.1631768207306/1000</f>
+        <v>1.0163176820730599E-2</v>
+      </c>
+      <c r="G45" s="2">
+        <f>20.97/1000</f>
+        <v>2.0969999999999999E-2</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1CB86B-8C48-416D-A7E1-B75D92C9D066}">
+  <dimension ref="A1:M60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" customWidth="1"/>
+    <col min="6" max="10" width="14" customWidth="1"/>
+    <col min="11" max="12" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="B32" s="12">
         <v>2017</v>
       </c>
@@ -1529,11 +2307,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C6DC6-3707-4513-B1FF-6845D503F7DD}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -2349,7 +3127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBC329E-241C-41A9-AB46-60A0479CEBAF}">
   <dimension ref="A1:M60"/>
   <sheetViews>
@@ -3159,11 +3937,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C407C159-8904-44D0-B7C7-833315191BBC}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -3962,11 +4740,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735D713C-0288-4607-850D-121F4BB78710}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -5073,12 +5851,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA16AE9-162C-4BF3-B3D7-7E425583483C}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6198,11 +6976,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428C295-1449-B942-94DE-B4DC493F45AE}">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="B33" workbookViewId="0">
       <selection activeCell="O18" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
@@ -7414,11 +8192,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3228D5-8C52-004C-AB7F-D57B454DC51F}">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>

</xml_diff>